<commit_message>
Fixed bug of user roles edit and add
</commit_message>
<xml_diff>
--- a/prototype/templates/user_department_template.xlsx
+++ b/prototype/templates/user_department_template.xlsx
@@ -490,7 +490,16 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
+  <dataValidations count="13">
+    <dataValidation sqref="F2:F100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"Male,Female,Unspecified"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"Dr,Mr,Ms,Prof,Rev"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
+      <formula1>"Fine,Not Fine"</formula1>
+    </dataValidation>
     <dataValidation sqref="F2:F100" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="list">
       <formula1>"Male,Female,Unspecified"</formula1>
     </dataValidation>
@@ -602,7 +611,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Department of Computer ScienceDepartment of Computer ScienceDepartment of Computer ScienceDepartment of Computer ScienceDepartment of Computer ScienceDepartment of Computer Science</t>
+          <t>Department of Computer Science</t>
         </is>
       </c>
     </row>

</xml_diff>